<commit_message>
add some content and some data
</commit_message>
<xml_diff>
--- a/data/dinner-club-history.xlsx
+++ b/data/dinner-club-history.xlsx
@@ -36,9 +36,6 @@
     <t xml:space="preserve"> Jeff</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sarah H</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Kevin Y</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sara H</t>
   </si>
 </sst>
 </file>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,27 +563,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -591,7 +591,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -631,71 +631,71 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
@@ -703,7 +703,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
@@ -711,71 +711,71 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
@@ -783,15 +783,15 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s">
         <v>3</v>
@@ -807,39 +807,39 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
@@ -855,26 +855,26 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>